<commit_message>
docs: updt Formulas hoja de personal y general
</commit_message>
<xml_diff>
--- a/frm_Costos v1.0.xlsx
+++ b/frm_Costos v1.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie-chan\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie-chan\Documents\GitHub\20220308-Formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BA8EE4-A328-4482-A73C-DF65BD8DB935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2A6FF6-099D-4D58-BC70-338B51A49B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{798AAD7E-BDD1-4553-9CF1-ACC7B624A934}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{798AAD7E-BDD1-4553-9CF1-ACC7B624A934}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMACION GENERAL" sheetId="8" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="77">
   <si>
     <t>PROYECTO</t>
   </si>
@@ -241,9 +241,6 @@
     <t>EXTRA</t>
   </si>
   <si>
-    <t>ID EMP</t>
-  </si>
-  <si>
     <t>NOMBRE</t>
   </si>
   <si>
@@ -271,12 +268,6 @@
     <t>Baja</t>
   </si>
   <si>
-    <t>JCBT</t>
-  </si>
-  <si>
-    <t>DEV</t>
-  </si>
-  <si>
     <t>PRECIO</t>
   </si>
   <si>
@@ -299,6 +290,27 @@
   </si>
   <si>
     <t>Proyecto c</t>
+  </si>
+  <si>
+    <t>ETIQUETA</t>
+  </si>
+  <si>
+    <t>Lider de Proyecto</t>
+  </si>
+  <si>
+    <t>Administrativo</t>
+  </si>
+  <si>
+    <t>TIEMPO MUERTO</t>
+  </si>
+  <si>
+    <t>APROX</t>
+  </si>
+  <si>
+    <t>PERSONA NUMERO UNO</t>
+  </si>
+  <si>
+    <t>pnu@example.com</t>
   </si>
 </sst>
 </file>
@@ -308,7 +320,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,8 +356,23 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,8 +409,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="52">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -902,163 +935,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="3"/>
-      </left>
-      <right style="dotted">
-        <color theme="3"/>
-      </right>
-      <top style="thin">
-        <color theme="3"/>
-      </top>
-      <bottom style="dotted">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color theme="3"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="3"/>
-      </top>
-      <bottom style="dotted">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color theme="3"/>
-      </left>
-      <right style="thin">
-        <color theme="3"/>
-      </right>
-      <top style="thin">
-        <color theme="3"/>
-      </top>
-      <bottom style="dotted">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3"/>
-      </left>
-      <right style="dotted">
-        <color theme="3"/>
-      </right>
-      <top style="dotted">
-        <color theme="3"/>
-      </top>
-      <bottom style="dotted">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color theme="3"/>
-      </left>
-      <right style="thin">
-        <color theme="3"/>
-      </right>
-      <top style="dotted">
-        <color theme="3"/>
-      </top>
-      <bottom style="dotted">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3"/>
-      </left>
-      <right style="dotted">
-        <color theme="3"/>
-      </right>
-      <top style="dotted">
-        <color theme="3"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color theme="3"/>
-      </left>
-      <right style="dotted">
-        <color theme="3"/>
-      </right>
-      <top style="dotted">
-        <color theme="3"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color theme="3"/>
-      </left>
-      <right/>
-      <top style="dotted">
-        <color theme="3"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color theme="3"/>
-      </left>
-      <right style="thin">
-        <color theme="3"/>
-      </right>
-      <top style="dotted">
-        <color theme="3"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3"/>
-      </left>
-      <right style="dotted">
-        <color theme="3"/>
-      </right>
-      <top style="dotted">
-        <color theme="3"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color theme="3"/>
-      </left>
-      <right style="thin">
-        <color theme="3"/>
-      </right>
-      <top style="dotted">
-        <color theme="3"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="mediumDashed">
         <color theme="3"/>
       </left>
@@ -1085,10 +961,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1188,37 +1065,16 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1253,7 +1109,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1289,11 +1145,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="6" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="73">
+  <dxfs count="89">
     <dxf>
       <font>
         <b val="0"/>
@@ -1306,7 +1183,126 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color auto="1"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
+        <right/>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom style="dotted">
+          <color theme="3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom style="dotted">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
+        <right/>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom style="dotted">
+          <color theme="3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Calibri Light"/>
         <family val="2"/>
         <scheme val="major"/>
@@ -1315,11 +1311,11 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="dotted">
           <color theme="3"/>
         </left>
@@ -1329,7 +1325,15 @@
         <top style="dotted">
           <color theme="3"/>
         </top>
-        <bottom/>
+        <bottom style="dotted">
+          <color theme="3"/>
+        </bottom>
+        <vertical style="dotted">
+          <color theme="3"/>
+        </vertical>
+        <horizontal style="dotted">
+          <color theme="3"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1349,186 +1353,7 @@
         <family val="2"/>
         <scheme val="major"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="dotted">
-          <color theme="3"/>
-        </left>
-        <right style="dotted">
-          <color theme="3"/>
-        </right>
-        <top style="dotted">
-          <color theme="3"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="dotted">
-          <color theme="3"/>
-        </left>
-        <right style="dotted">
-          <color theme="3"/>
-        </right>
-        <top style="dotted">
-          <color theme="3"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="dotted">
-          <color theme="3"/>
-        </left>
-        <right style="dotted">
-          <color theme="3"/>
-        </right>
-        <top style="dotted">
-          <color theme="3"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="dotted">
-          <color theme="3"/>
-        </left>
-        <right style="dotted">
-          <color theme="3"/>
-        </right>
-        <top style="dotted">
-          <color theme="3"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="dotted">
-          <color theme="3"/>
-        </left>
-        <right style="dotted">
-          <color theme="3"/>
-        </right>
-        <top style="dotted">
-          <color theme="3"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1540,6 +1365,186 @@
         <left style="dotted">
           <color theme="3"/>
         </left>
+        <right style="thick">
+          <color rgb="FF6096BA"/>
+        </right>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
+        <right style="dotted">
+          <color theme="3"/>
+        </right>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
+        <right style="dotted">
+          <color theme="3"/>
+        </right>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
+        <right style="dotted">
+          <color theme="3"/>
+        </right>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
+        <right style="dotted">
+          <color theme="3"/>
+        </right>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
         <right style="dotted">
           <color theme="3"/>
         </right>
@@ -1683,6 +1688,43 @@
           <bgColor theme="3" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
+        <right style="dotted">
+          <color theme="3"/>
+        </right>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="dotted">
           <color theme="3"/>
@@ -1909,6 +1951,439 @@
           <color theme="3"/>
         </top>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
+        <right style="dotted">
+          <color theme="3"/>
+        </right>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom style="dotted">
+          <color theme="3"/>
+        </bottom>
+        <vertical style="dotted">
+          <color theme="3"/>
+        </vertical>
+        <horizontal style="dotted">
+          <color theme="3"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
+        <right style="dotted">
+          <color theme="3"/>
+        </right>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom style="dotted">
+          <color theme="3"/>
+        </bottom>
+        <vertical style="dotted">
+          <color theme="3"/>
+        </vertical>
+        <horizontal style="dotted">
+          <color theme="3"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
+        <right style="dotted">
+          <color theme="3"/>
+        </right>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom style="dotted">
+          <color theme="3"/>
+        </bottom>
+        <vertical style="dotted">
+          <color theme="3"/>
+        </vertical>
+        <horizontal style="dotted">
+          <color theme="3"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
+        <right style="dotted">
+          <color theme="3"/>
+        </right>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom style="dotted">
+          <color theme="3"/>
+        </bottom>
+        <vertical style="dotted">
+          <color theme="3"/>
+        </vertical>
+        <horizontal style="dotted">
+          <color theme="3"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
+        <right style="dotted">
+          <color theme="3"/>
+        </right>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom style="dotted">
+          <color theme="3"/>
+        </bottom>
+        <vertical style="dotted">
+          <color theme="3"/>
+        </vertical>
+        <horizontal style="dotted">
+          <color theme="3"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
+        <right style="dotted">
+          <color theme="3"/>
+        </right>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom style="dotted">
+          <color theme="3"/>
+        </bottom>
+        <vertical style="dotted">
+          <color theme="3"/>
+        </vertical>
+        <horizontal style="dotted">
+          <color theme="3"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color theme="3"/>
+        </left>
+        <right style="dotted">
+          <color theme="3"/>
+        </right>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom style="dotted">
+          <color theme="3"/>
+        </bottom>
+        <vertical style="dotted">
+          <color theme="3"/>
+        </vertical>
+        <horizontal style="dotted">
+          <color theme="3"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="dotted">
+          <color theme="3"/>
+        </right>
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+        <bottom style="dotted">
+          <color theme="3"/>
+        </bottom>
+        <vertical style="dotted">
+          <color theme="3"/>
+        </vertical>
+        <horizontal style="dotted">
+          <color theme="3"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="dotted">
+          <color theme="3"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="dotted">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2963,52 +3438,6 @@
         <bottom style="dotted">
           <color theme="3"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dotted">
-          <color theme="3"/>
-        </left>
-        <right style="thick">
-          <color rgb="FF6096BA"/>
-        </right>
-        <top style="dotted">
-          <color theme="3"/>
-        </top>
-        <bottom style="dotted">
-          <color theme="3"/>
-        </bottom>
-        <vertical style="dotted">
-          <color theme="3"/>
-        </vertical>
-        <horizontal style="dotted">
-          <color theme="3"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -3831,11 +4260,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3851,35 +4275,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{152D9D78-16FE-46AF-9964-5FBE7B7079C0}" name="tbl_InformacionGeneral" displayName="tbl_InformacionGeneral" ref="B3:R13" totalsRowCount="1" headerRowDxfId="71" dataDxfId="69" totalsRowDxfId="67" headerRowBorderDxfId="70" tableBorderDxfId="68" totalsRowBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{152D9D78-16FE-46AF-9964-5FBE7B7079C0}" name="tbl_InformacionGeneral" displayName="tbl_InformacionGeneral" ref="B3:R13" totalsRowCount="1" headerRowDxfId="88" dataDxfId="86" totalsRowDxfId="84" headerRowBorderDxfId="87" tableBorderDxfId="85" totalsRowBorderDxfId="83">
   <autoFilter ref="B3:R12" xr:uid="{152D9D78-16FE-46AF-9964-5FBE7B7079C0}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{38264488-2A35-4569-959A-87AF45BA57B2}" name="ID" totalsRowLabel="Total" dataDxfId="65" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{07DE2906-B456-4045-9071-23477BEAB3BD}" name="NOMBRE PROYECTO" dataDxfId="64" totalsRowDxfId="15"/>
-    <tableColumn id="15" xr3:uid="{5C4019C8-53AE-4B1B-B8F4-59313202B1DB}" name="GANANCIA BRUTA" totalsRowFunction="sum" dataDxfId="63" totalsRowDxfId="14">
+    <tableColumn id="1" xr3:uid="{38264488-2A35-4569-959A-87AF45BA57B2}" name="ID" totalsRowLabel="Total" dataDxfId="82" totalsRowDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{07DE2906-B456-4045-9071-23477BEAB3BD}" name="NOMBRE PROYECTO" dataDxfId="81" totalsRowDxfId="20"/>
+    <tableColumn id="15" xr3:uid="{5C4019C8-53AE-4B1B-B8F4-59313202B1DB}" name="GANANCIA BRUTA" totalsRowFunction="sum" dataDxfId="80" totalsRowDxfId="19">
       <calculatedColumnFormula>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{9133F0CA-4FB3-4A2D-A7C3-45424DFC4880}" name="MARGEN R" dataDxfId="62" totalsRowDxfId="13">
+    <tableColumn id="19" xr3:uid="{9133F0CA-4FB3-4A2D-A7C3-45424DFC4880}" name="MARGEN R" dataDxfId="79" totalsRowDxfId="18">
       <calculatedColumnFormula>IF(tbl_InformacionGeneral[[#This Row],[PRECIO]],IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,tbl_InformacionGeneral[[#This Row],[GANANCIA BRUTA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]],tbl_InformacionGeneral[[#This Row],[PERDIDA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]]),"Sin datos")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C7AA8410-EB51-4033-A690-0EFA69D14174}" name="PERDIDA" dataDxfId="61" totalsRowDxfId="12">
+    <tableColumn id="4" xr3:uid="{C7AA8410-EB51-4033-A690-0EFA69D14174}" name="PERDIDA" dataDxfId="78" totalsRowDxfId="17">
       <calculatedColumnFormula>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&lt;0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{103AD4B0-4E9E-46B1-8869-E99D5FF6C997}" name="FECHA INICIAL E" dataDxfId="60" totalsRowDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{F59D9D85-8466-4808-B818-CD46A14B8DD4}" name="FECHA FINAL E" dataDxfId="59" totalsRowDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{3FBF59AD-2E21-4CD8-AA6D-7FB271A39EC6}" name="DIAS E" dataDxfId="58" totalsRowDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{8FEB0B58-42A5-422C-A4D9-50799175F132}" name="RECURSOS E" dataDxfId="57" totalsRowDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{01AF3C88-C89B-44D1-9E48-B76FCC3E16B0}" name="COSTO" dataDxfId="56" totalsRowDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{CC5BABAD-DB88-45B9-9629-7C2A36C0AFBE}" name="MARGEN B" dataDxfId="55" totalsRowDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{E2EA7E82-3B24-4E14-BA28-76CF2E2CABA5}" name="PRECIO" dataDxfId="54" totalsRowDxfId="5">
+    <tableColumn id="5" xr3:uid="{103AD4B0-4E9E-46B1-8869-E99D5FF6C997}" name="FECHA INICIAL E" dataDxfId="77" totalsRowDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{F59D9D85-8466-4808-B818-CD46A14B8DD4}" name="FECHA FINAL E" dataDxfId="76" totalsRowDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{3FBF59AD-2E21-4CD8-AA6D-7FB271A39EC6}" name="DIAS E" dataDxfId="75" totalsRowDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{8FEB0B58-42A5-422C-A4D9-50799175F132}" name="RECURSOS E" dataDxfId="74" totalsRowDxfId="13"/>
+    <tableColumn id="18" xr3:uid="{01AF3C88-C89B-44D1-9E48-B76FCC3E16B0}" name="COSTO" dataDxfId="73" totalsRowDxfId="12"/>
+    <tableColumn id="17" xr3:uid="{CC5BABAD-DB88-45B9-9629-7C2A36C0AFBE}" name="MARGEN B" dataDxfId="72" totalsRowDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{E2EA7E82-3B24-4E14-BA28-76CF2E2CABA5}" name="PRECIO" dataDxfId="71" totalsRowDxfId="10">
       <calculatedColumnFormula>IF(tbl_InformacionGeneral[[#This Row],[COSTO]]&gt;0,tbl_InformacionGeneral[[#This Row],[COSTO]]/(1-tbl_InformacionGeneral[[#This Row],[MARGEN B]]),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{2A6B102E-6E1A-48E9-A868-C8BC8D7CD5BD}" name="FECHA INICIAL R" dataDxfId="53" totalsRowDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{3518D165-CFA4-4C06-A0F8-C83CFEC0B138}" name="FECHA FINALR" dataDxfId="52" totalsRowDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{7910CE3E-3E22-479D-A998-A4077FE6AF3D}" name="DIAS R" dataDxfId="51" totalsRowDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{E2A5524C-A317-4B1B-BEE6-0F0F400A7A73}" name="RECURSOS R" dataDxfId="50" totalsRowDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{89E4A1D2-92FF-4FE1-A6A9-E6BD331734EC}" name="COSTO REAL" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="0">
-      <calculatedColumnFormula array="1">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],tbl_Asignaciones[COSTO TOTAL],0)),0)</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{2A6B102E-6E1A-48E9-A868-C8BC8D7CD5BD}" name="FECHA INICIAL R" dataDxfId="70" totalsRowDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{3518D165-CFA4-4C06-A0F8-C83CFEC0B138}" name="FECHA FINALR" dataDxfId="69" totalsRowDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{7910CE3E-3E22-479D-A998-A4077FE6AF3D}" name="DIAS R" dataDxfId="68" totalsRowDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{E2A5524C-A317-4B1B-BEE6-0F0F400A7A73}" name="RECURSOS R" dataDxfId="67" totalsRowDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{89E4A1D2-92FF-4FE1-A6A9-E6BD331734EC}" name="COSTO REAL" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5">
+      <calculatedColumnFormula array="1">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],IF(tbl_Asignaciones[OFICIAL]="Y",tbl_Asignaciones[COSTO TOTAL],0),0)),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3887,44 +4311,87 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C8512D0-C502-4456-9E96-2DACE5D29A28}" name="tbl_Asignaciones" displayName="tbl_Asignaciones" ref="B2:M33" totalsRowShown="0" headerRowBorderDxfId="48" tableBorderDxfId="47" totalsRowBorderDxfId="46">
-  <autoFilter ref="B2:M33" xr:uid="{8C8512D0-C502-4456-9E96-2DACE5D29A28}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C8512D0-C502-4456-9E96-2DACE5D29A28}" name="tbl_Asignaciones" displayName="tbl_Asignaciones" ref="B2:M32" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65" totalsRowBorderDxfId="64">
+  <autoFilter ref="B2:M32" xr:uid="{8C8512D0-C502-4456-9E96-2DACE5D29A28}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{EABBD557-1FD0-46CD-A273-8138C5F05307}" name="ID" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{C268D762-85B7-4E17-A674-FB666B2389D6}" name="NOMBRE PROYECTO" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{892EB1D5-4837-4F08-B7C7-361A40E04014}" name="ASIGNACION" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{0E1B21F7-B6C2-469C-8C59-642B22A4343D}" name="OFICIAL" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{CEDACCDC-917D-47DD-B6C2-DE588AC32D1F}" name="FECHA DE INICIO" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{AD9B95F6-EDE8-42B7-B070-B1FA18D53F41}" name="FECHA FINAL" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{275D946C-F89A-499B-ACA1-B9AF42BDBE31}" name="DIAS" dataDxfId="39"/>
-    <tableColumn id="8" xr3:uid="{D6D8E3A9-7D78-45EF-AAAB-2E91A1596ECE}" name="HRS" dataDxfId="38"/>
-    <tableColumn id="9" xr3:uid="{737301BA-0471-4738-A488-D4C192801012}" name="COSTO" dataDxfId="37"/>
-    <tableColumn id="10" xr3:uid="{408CB203-AC14-4093-A9E7-15E53DE15678}" name="TARIFA" dataDxfId="36"/>
-    <tableColumn id="11" xr3:uid="{E3B5E482-DD6E-4706-8F9E-3F2B2D334201}" name="EXTRA" dataDxfId="35"/>
-    <tableColumn id="12" xr3:uid="{20A71CC6-4064-412D-AABD-7D2484D18C4B}" name="COSTO TOTAL" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{EABBD557-1FD0-46CD-A273-8138C5F05307}" name="ID" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{C268D762-85B7-4E17-A674-FB666B2389D6}" name="NOMBRE PROYECTO" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{892EB1D5-4837-4F08-B7C7-361A40E04014}" name="ASIGNACION" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{0E1B21F7-B6C2-469C-8C59-642B22A4343D}" name="OFICIAL" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{CEDACCDC-917D-47DD-B6C2-DE588AC32D1F}" name="FECHA DE INICIO" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{AD9B95F6-EDE8-42B7-B070-B1FA18D53F41}" name="FECHA FINAL" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{275D946C-F89A-499B-ACA1-B9AF42BDBE31}" name="DIAS" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{D6D8E3A9-7D78-45EF-AAAB-2E91A1596ECE}" name="HRS" dataDxfId="56"/>
+    <tableColumn id="9" xr3:uid="{737301BA-0471-4738-A488-D4C192801012}" name="COSTO" dataDxfId="55"/>
+    <tableColumn id="10" xr3:uid="{408CB203-AC14-4093-A9E7-15E53DE15678}" name="TARIFA" dataDxfId="54"/>
+    <tableColumn id="11" xr3:uid="{E3B5E482-DD6E-4706-8F9E-3F2B2D334201}" name="EXTRA" dataDxfId="53"/>
+    <tableColumn id="12" xr3:uid="{20A71CC6-4064-412D-AABD-7D2484D18C4B}" name="COSTO TOTAL" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A15356D-E9EE-426B-995B-2923B1AF1D74}" name="tbl_DatosGenerale" displayName="tbl_DatosGenerale" ref="B2:M12" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{02D7EA06-3588-4F69-B8FA-E55885444D7C}" name="tbl_Personal" displayName="tbl_Personal" ref="B2:L8" totalsRowShown="0" headerRowDxfId="30" dataDxfId="31" headerRowBorderDxfId="33" tableBorderDxfId="34" totalsRowBorderDxfId="32">
+  <autoFilter ref="B2:L8" xr:uid="{02D7EA06-3588-4F69-B8FA-E55885444D7C}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{9089348E-1096-4169-A5A3-486F957894FD}" name="ETIQUETA" dataDxfId="29">
+      <calculatedColumnFormula>CHOOSE(
+LEN(tbl_Personal[[#This Row],[NOMBRE]]) - LEN(SUBSTITUTE(tbl_Personal[[#This Row],[NOMBRE]]," ","")) + 1,
+LEFT(tbl_Personal[[#This Row],[NOMBRE]]),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1) + 1, 1))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{942CEB41-2058-473B-B50B-7067440916DF}" name="NOMBRE" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{5F1A71F5-3CD9-4CCB-899C-B9F487EE30C1}" name="ROL" dataDxfId="27">
+      <calculatedColumnFormula>CHOOSE(
+LEN(tbl_Personal[[#This Row],[NOMBRE]]) - LEN(SUBSTITUTE(tbl_Personal[[#This Row],[NOMBRE]]," ","")) + 1,
+LEFT(tbl_Personal[[#This Row],[NOMBRE]]),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{DF69F488-7E29-4634-A5AC-44A74B1FA0D3}" name="CORREO" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{7FA6FAA8-A2C6-410D-A457-4AE03B39521B}" name="ESTADO" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{306D3F81-09E2-4490-8017-D05836182563}" name="N° PROYECTOS ASIGNADO" dataDxfId="24">
+      <calculatedColumnFormula>COUNTIF(tbl_Asignaciones[ASIGNACION],tbl_Personal[[#This Row],[NOMBRE]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{74FC653F-F16B-40D8-9800-AD771C1735BC}" name="FECHA INICIAL" dataDxfId="23">
+      <calculatedColumnFormula array="1">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",MIN(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA DE INICIO]," "))," ")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{08287A6D-5215-4A90-8269-E95CB3F4D252}" name="FECHA FINAL" dataDxfId="22">
+      <calculatedColumnFormula array="1">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",MAX(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA FINAL]," "))," ")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{5FF784A2-B247-4976-95BE-52316B99AF8E}" name="APROX" dataDxfId="3">
+      <calculatedColumnFormula array="1">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",NETWORKDAYS.INTL(MIN(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA FINAL]," ")),MAX(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA DE INICIO]," ")),1)-2," ")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{861FC0B2-B263-41D9-88A2-031068086C27}" name="DIAS" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{B3D6CEFD-1DFD-45F1-8D59-5C8A8089C830}" name="TIEMPO MUERTO" dataDxfId="2">
+      <calculatedColumnFormula>IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",IF(tbl_Personal[[#This Row],[APROX]]&gt;0,"SI","NO"),"")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A15356D-E9EE-426B-995B-2923B1AF1D74}" name="tbl_DatosGenerale" displayName="tbl_DatosGenerale" ref="B2:M12" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48" totalsRowBorderDxfId="47">
   <autoFilter ref="B2:M12" xr:uid="{7A15356D-E9EE-426B-995B-2923B1AF1D74}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{AD88CAB9-A51E-4111-A18D-7F7DF6FDCB08}" name="ID" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{DA2B770F-1215-4EC2-AE48-1007D9DE0F08}" name="PROYECTO" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{4EA14D83-C8F4-4FDC-92EA-762D861D3B5B}" name="RECURSOS" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{0E552704-E335-43D6-AD86-56257766D811}" name="FECHA DE INICIO" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{53289D6F-095F-4F4F-81F1-075CD512CFA7}" name="FECHA FINAL" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{3FEBB88D-DDD0-4ED7-A00D-7214F4B86202}" name="DIAS EXTRA" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{401D72DC-ADE3-46FF-9260-E58A22E0C449}" name="DIAS LAB" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{AD88CAB9-A51E-4111-A18D-7F7DF6FDCB08}" name="ID" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{DA2B770F-1215-4EC2-AE48-1007D9DE0F08}" name="PROYECTO" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{4EA14D83-C8F4-4FDC-92EA-762D861D3B5B}" name="RECURSOS" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{0E552704-E335-43D6-AD86-56257766D811}" name="FECHA DE INICIO" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{53289D6F-095F-4F4F-81F1-075CD512CFA7}" name="FECHA FINAL" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{3FEBB88D-DDD0-4ED7-A00D-7214F4B86202}" name="DIAS EXTRA" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{401D72DC-ADE3-46FF-9260-E58A22E0C449}" name="DIAS LAB" dataDxfId="40">
       <calculatedColumnFormula>NETWORKDAYS(tbl_DatosGenerale[[#This Row],[FECHA DE INICIO]],tbl_DatosGenerale[[#This Row],[FECHA FINAL]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5827EADF-41C5-4FBD-9B54-FA65E9FD7B05}" name="OFICIAL" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{5BEB8603-1730-494F-82FC-3D40DB3EF217}" name="COSTO" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{4E33FA01-01F3-4BFF-B99E-9EA3005805F9}" name="HRS" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{FBF4A668-D475-4D94-9DF3-F9A26844661D}" name="TARIFA" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{7532AA04-9B0E-417E-A89B-9E338DEC6998}" name="COSTO TOTAL" dataDxfId="17">
+    <tableColumn id="10" xr3:uid="{5827EADF-41C5-4FBD-9B54-FA65E9FD7B05}" name="OFICIAL" dataDxfId="39"/>
+    <tableColumn id="8" xr3:uid="{5BEB8603-1730-494F-82FC-3D40DB3EF217}" name="COSTO" dataDxfId="38"/>
+    <tableColumn id="11" xr3:uid="{4E33FA01-01F3-4BFF-B99E-9EA3005805F9}" name="HRS" dataDxfId="37"/>
+    <tableColumn id="12" xr3:uid="{FBF4A668-D475-4D94-9DF3-F9A26844661D}" name="TARIFA" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{7532AA04-9B0E-417E-A89B-9E338DEC6998}" name="COSTO TOTAL" dataDxfId="35">
       <calculatedColumnFormula>((tbl_DatosGenerale[[#This Row],[COSTO]]*tbl_DatosGenerale[[#This Row],[HRS]])*tbl_DatosGenerale[[#This Row],[DIAS LAB]])+((tbl_DatosGenerale[[#This Row],[COSTO]]*tbl_DatosGenerale[[#This Row],[HRS]])*tbl_DatosGenerale[[#This Row],[DIAS EXTRA]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4231,9 +4698,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{634F5700-8FC9-4E9B-B45F-7ECFDBD4BE16}">
   <dimension ref="B1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="6" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O6" sqref="O6"/>
+      <selection pane="topRight" activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4242,14 +4709,14 @@
     <col min="2" max="2" width="8.21875" style="50" customWidth="1"/>
     <col min="3" max="3" width="39.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.109375" style="59" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="79" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="66" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" style="59" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" style="51" customWidth="1"/>
     <col min="10" max="10" width="11.88671875" style="55" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" style="74" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" style="76" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" style="61" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" style="63" customWidth="1"/>
     <col min="13" max="13" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" style="1" customWidth="1"/>
     <col min="15" max="15" width="14.6640625" style="1" customWidth="1"/>
@@ -4261,29 +4728,29 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="90" t="s">
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="94" t="s">
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="94"/>
-      <c r="P2" s="94"/>
-      <c r="Q2" s="94"/>
-      <c r="R2" s="95"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="82"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="57" t="s">
@@ -4292,11 +4759,11 @@
       <c r="C3" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="80" t="s">
-        <v>66</v>
+      <c r="D3" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="67" t="s">
+        <v>63</v>
       </c>
       <c r="F3" s="60" t="s">
         <v>36</v>
@@ -4313,14 +4780,14 @@
       <c r="J3" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="75" t="s">
+      <c r="K3" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="77" t="s">
-        <v>68</v>
+      <c r="L3" s="64" t="s">
+        <v>65</v>
       </c>
       <c r="M3" s="47" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N3" s="46" t="s">
         <v>46</v>
@@ -4343,21 +4810,21 @@
         <v>38</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4" s="12">
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
-        <v>87700</v>
-      </c>
-      <c r="E4" s="81">
+        <v>88000</v>
+      </c>
+      <c r="E4" s="68">
         <f>IF(tbl_InformacionGeneral[[#This Row],[PRECIO]],IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,tbl_InformacionGeneral[[#This Row],[GANANCIA BRUTA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]],tbl_InformacionGeneral[[#This Row],[PERDIDA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]]),"Sin datos")</f>
-        <v>0.877</v>
+        <v>0.88</v>
       </c>
       <c r="F4" s="12">
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&lt;0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="82">
+      <c r="G4" s="69">
         <v>44593</v>
       </c>
       <c r="H4" s="10">
@@ -4370,10 +4837,10 @@
       <c r="J4" s="53">
         <v>5</v>
       </c>
-      <c r="K4" s="83">
+      <c r="K4" s="70">
         <v>50000</v>
       </c>
-      <c r="L4" s="84">
+      <c r="L4" s="71">
         <v>0.5</v>
       </c>
       <c r="M4" s="12">
@@ -4381,12 +4848,12 @@
         <v>100000</v>
       </c>
       <c r="N4" s="12"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="68"/>
+      <c r="Q4" s="68"/>
       <c r="R4" s="43" cm="1">
-        <f t="array" ref="R4">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],tbl_Asignaciones[COSTO TOTAL],0)),0)</f>
-        <v>12300</v>
+        <f t="array" ref="R4">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],IF(tbl_Asignaciones[OFICIAL]="Y",tbl_Asignaciones[COSTO TOTAL],0),0)),0)</f>
+        <v>12000</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
@@ -4394,21 +4861,21 @@
         <v>39</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D5" s="12">
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="81">
+        <v>11111.111111111111</v>
+      </c>
+      <c r="E5" s="68">
         <f>IF(tbl_InformacionGeneral[[#This Row],[PRECIO]],IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,tbl_InformacionGeneral[[#This Row],[GANANCIA BRUTA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]],tbl_InformacionGeneral[[#This Row],[PERDIDA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]]),"Sin datos")</f>
-        <v>-0.89</v>
+        <v>1</v>
       </c>
       <c r="F5" s="12">
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&lt;0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
-        <v>-9888.8888888888887</v>
-      </c>
-      <c r="G5" s="82">
+        <v>0</v>
+      </c>
+      <c r="G5" s="69">
         <v>44607</v>
       </c>
       <c r="H5" s="10">
@@ -4421,10 +4888,10 @@
       <c r="J5" s="53">
         <v>3</v>
       </c>
-      <c r="K5" s="83">
+      <c r="K5" s="70">
         <v>10000</v>
       </c>
-      <c r="L5" s="84">
+      <c r="L5" s="71">
         <v>0.1</v>
       </c>
       <c r="M5" s="12">
@@ -4432,12 +4899,12 @@
         <v>11111.111111111111</v>
       </c>
       <c r="N5" s="12"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="68"/>
+      <c r="Q5" s="68"/>
       <c r="R5" s="43" cm="1">
-        <f t="array" ref="R5">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],tbl_Asignaciones[COSTO TOTAL],0)),0)</f>
-        <v>21000</v>
+        <f t="array" ref="R5">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],IF(tbl_Asignaciones[OFICIAL]="Y",tbl_Asignaciones[COSTO TOTAL],0),0)),0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
@@ -4445,13 +4912,13 @@
         <v>41</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D6" s="12">
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>80</v>
       </c>
-      <c r="E6" s="81">
+      <c r="E6" s="68">
         <f>IF(tbl_InformacionGeneral[[#This Row],[PRECIO]],IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,tbl_InformacionGeneral[[#This Row],[GANANCIA BRUTA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]],tbl_InformacionGeneral[[#This Row],[PERDIDA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]]),"Sin datos")</f>
         <v>1</v>
       </c>
@@ -4459,7 +4926,7 @@
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&lt;0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="82">
+      <c r="G6" s="69">
         <v>44613</v>
       </c>
       <c r="H6" s="10">
@@ -4472,10 +4939,10 @@
       <c r="J6" s="53">
         <v>2</v>
       </c>
-      <c r="K6" s="83">
+      <c r="K6" s="70">
         <v>45</v>
       </c>
-      <c r="L6" s="84">
+      <c r="L6" s="71">
         <v>0.4375</v>
       </c>
       <c r="M6" s="12">
@@ -4483,11 +4950,11 @@
         <v>80</v>
       </c>
       <c r="N6" s="12"/>
-      <c r="O6" s="81"/>
-      <c r="P6" s="81"/>
-      <c r="Q6" s="81"/>
+      <c r="O6" s="68"/>
+      <c r="P6" s="68"/>
+      <c r="Q6" s="68"/>
       <c r="R6" s="43" cm="1">
-        <f t="array" ref="R6">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],tbl_Asignaciones[COSTO TOTAL],0)),0)</f>
+        <f t="array" ref="R6">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],IF(tbl_Asignaciones[OFICIAL]="Y",tbl_Asignaciones[COSTO TOTAL],0),0)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4498,7 +4965,7 @@
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="81" t="str">
+      <c r="E7" s="68" t="str">
         <f>IF(tbl_InformacionGeneral[[#This Row],[PRECIO]],IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,tbl_InformacionGeneral[[#This Row],[GANANCIA BRUTA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]],tbl_InformacionGeneral[[#This Row],[PERDIDA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]]),"Sin datos")</f>
         <v>Sin datos</v>
       </c>
@@ -4506,14 +4973,14 @@
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&lt;0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="82"/>
+      <c r="G7" s="69"/>
       <c r="H7" s="10"/>
       <c r="I7" s="53"/>
       <c r="J7" s="53"/>
-      <c r="K7" s="83">
+      <c r="K7" s="70">
         <v>0</v>
       </c>
-      <c r="L7" s="84">
+      <c r="L7" s="71">
         <v>0</v>
       </c>
       <c r="M7" s="12">
@@ -4521,11 +4988,11 @@
         <v>0</v>
       </c>
       <c r="N7" s="12"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="81"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="68"/>
+      <c r="Q7" s="68"/>
       <c r="R7" s="43" cm="1">
-        <f t="array" ref="R7">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],tbl_Asignaciones[COSTO TOTAL],0)),0)</f>
+        <f t="array" ref="R7">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],IF(tbl_Asignaciones[OFICIAL]="Y",tbl_Asignaciones[COSTO TOTAL],0),0)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4536,7 +5003,7 @@
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="81" t="str">
+      <c r="E8" s="68" t="str">
         <f>IF(tbl_InformacionGeneral[[#This Row],[PRECIO]],IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,tbl_InformacionGeneral[[#This Row],[GANANCIA BRUTA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]],tbl_InformacionGeneral[[#This Row],[PERDIDA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]]),"Sin datos")</f>
         <v>Sin datos</v>
       </c>
@@ -4544,22 +5011,22 @@
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&lt;0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="82"/>
+      <c r="G8" s="69"/>
       <c r="H8" s="10"/>
       <c r="I8" s="53"/>
       <c r="J8" s="53"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="84"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="71"/>
       <c r="M8" s="12">
         <f>IF(tbl_InformacionGeneral[[#This Row],[COSTO]]&gt;0,tbl_InformacionGeneral[[#This Row],[COSTO]]/(1-tbl_InformacionGeneral[[#This Row],[MARGEN B]]),0)</f>
         <v>0</v>
       </c>
       <c r="N8" s="12"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="81"/>
-      <c r="Q8" s="81"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="68"/>
+      <c r="Q8" s="68"/>
       <c r="R8" s="43" cm="1">
-        <f t="array" ref="R8">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],tbl_Asignaciones[COSTO TOTAL],0)),0)</f>
+        <f t="array" ref="R8">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],IF(tbl_Asignaciones[OFICIAL]="Y",tbl_Asignaciones[COSTO TOTAL],0),0)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4570,7 +5037,7 @@
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="81" t="str">
+      <c r="E9" s="68" t="str">
         <f>IF(tbl_InformacionGeneral[[#This Row],[PRECIO]],IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,tbl_InformacionGeneral[[#This Row],[GANANCIA BRUTA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]],tbl_InformacionGeneral[[#This Row],[PERDIDA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]]),"Sin datos")</f>
         <v>Sin datos</v>
       </c>
@@ -4578,22 +5045,22 @@
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&lt;0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="82"/>
+      <c r="G9" s="69"/>
       <c r="H9" s="10"/>
       <c r="I9" s="53"/>
       <c r="J9" s="53"/>
-      <c r="K9" s="83"/>
-      <c r="L9" s="84"/>
+      <c r="K9" s="70"/>
+      <c r="L9" s="71"/>
       <c r="M9" s="12">
         <f>IF(tbl_InformacionGeneral[[#This Row],[COSTO]]&gt;0,tbl_InformacionGeneral[[#This Row],[COSTO]]/(1-tbl_InformacionGeneral[[#This Row],[MARGEN B]]),0)</f>
         <v>0</v>
       </c>
       <c r="N9" s="12"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="81"/>
-      <c r="Q9" s="81"/>
+      <c r="O9" s="68"/>
+      <c r="P9" s="68"/>
+      <c r="Q9" s="68"/>
       <c r="R9" s="43" cm="1">
-        <f t="array" ref="R9">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],tbl_Asignaciones[COSTO TOTAL],0)),0)</f>
+        <f t="array" ref="R9">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],IF(tbl_Asignaciones[OFICIAL]="Y",tbl_Asignaciones[COSTO TOTAL],0),0)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4604,7 +5071,7 @@
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="81" t="str">
+      <c r="E10" s="68" t="str">
         <f>IF(tbl_InformacionGeneral[[#This Row],[PRECIO]],IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,tbl_InformacionGeneral[[#This Row],[GANANCIA BRUTA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]],tbl_InformacionGeneral[[#This Row],[PERDIDA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]]),"Sin datos")</f>
         <v>Sin datos</v>
       </c>
@@ -4612,22 +5079,22 @@
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&lt;0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="82"/>
+      <c r="G10" s="69"/>
       <c r="H10" s="10"/>
       <c r="I10" s="54"/>
       <c r="J10" s="53"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="84"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="71"/>
       <c r="M10" s="12">
         <f>IF(tbl_InformacionGeneral[[#This Row],[COSTO]]&gt;0,tbl_InformacionGeneral[[#This Row],[COSTO]]/(1-tbl_InformacionGeneral[[#This Row],[MARGEN B]]),0)</f>
         <v>0</v>
       </c>
       <c r="N10" s="12"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
+      <c r="O10" s="68"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="68"/>
       <c r="R10" s="43" cm="1">
-        <f t="array" ref="R10">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],tbl_Asignaciones[COSTO TOTAL],0)),0)</f>
+        <f t="array" ref="R10">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],IF(tbl_Asignaciones[OFICIAL]="Y",tbl_Asignaciones[COSTO TOTAL],0),0)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4638,7 +5105,7 @@
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="81" t="str">
+      <c r="E11" s="68" t="str">
         <f>IF(tbl_InformacionGeneral[[#This Row],[PRECIO]],IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,tbl_InformacionGeneral[[#This Row],[GANANCIA BRUTA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]],tbl_InformacionGeneral[[#This Row],[PERDIDA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]]),"Sin datos")</f>
         <v>Sin datos</v>
       </c>
@@ -4646,22 +5113,22 @@
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&lt;0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="82"/>
+      <c r="G11" s="69"/>
       <c r="H11" s="10"/>
       <c r="I11" s="54"/>
       <c r="J11" s="53"/>
-      <c r="K11" s="83"/>
-      <c r="L11" s="84"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="71"/>
       <c r="M11" s="12">
         <f>IF(tbl_InformacionGeneral[[#This Row],[COSTO]]&gt;0,tbl_InformacionGeneral[[#This Row],[COSTO]]/(1-tbl_InformacionGeneral[[#This Row],[MARGEN B]]),0)</f>
         <v>0</v>
       </c>
       <c r="N11" s="12"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
+      <c r="O11" s="68"/>
+      <c r="P11" s="68"/>
+      <c r="Q11" s="68"/>
       <c r="R11" s="43" cm="1">
-        <f t="array" ref="R11">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],tbl_Asignaciones[COSTO TOTAL],0)),0)</f>
+        <f t="array" ref="R11">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],IF(tbl_Asignaciones[OFICIAL]="Y",tbl_Asignaciones[COSTO TOTAL],0),0)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4672,7 +5139,7 @@
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="81" t="str">
+      <c r="E12" s="68" t="str">
         <f>IF(tbl_InformacionGeneral[[#This Row],[PRECIO]],IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&gt;=0,tbl_InformacionGeneral[[#This Row],[GANANCIA BRUTA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]],tbl_InformacionGeneral[[#This Row],[PERDIDA]]/tbl_InformacionGeneral[[#This Row],[PRECIO]]),"Sin datos")</f>
         <v>Sin datos</v>
       </c>
@@ -4680,50 +5147,50 @@
         <f>IF((tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]])&lt;0,(tbl_InformacionGeneral[[#This Row],[PRECIO]]-tbl_InformacionGeneral[[#This Row],[COSTO REAL]]),0)</f>
         <v>0</v>
       </c>
-      <c r="G12" s="82"/>
+      <c r="G12" s="69"/>
       <c r="H12" s="10"/>
       <c r="I12" s="54"/>
       <c r="J12" s="53"/>
-      <c r="K12" s="83"/>
-      <c r="L12" s="84"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="71"/>
       <c r="M12" s="12">
         <f>IF(tbl_InformacionGeneral[[#This Row],[COSTO]]&gt;0,tbl_InformacionGeneral[[#This Row],[COSTO]]/(1-tbl_InformacionGeneral[[#This Row],[MARGEN B]]),0)</f>
         <v>0</v>
       </c>
       <c r="N12" s="12"/>
-      <c r="O12" s="81"/>
-      <c r="P12" s="81"/>
-      <c r="Q12" s="81"/>
+      <c r="O12" s="68"/>
+      <c r="P12" s="68"/>
+      <c r="Q12" s="68"/>
       <c r="R12" s="43" cm="1">
-        <f t="array" ref="R12">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],tbl_Asignaciones[COSTO TOTAL],0)),0)</f>
+        <f t="array" ref="R12">IFERROR(SUM(IF(tbl_Asignaciones[ID]=tbl_InformacionGeneral[[#This Row],[ID]],IF(tbl_Asignaciones[OFICIAL]="Y",tbl_Asignaciones[COSTO TOTAL],0),0)),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="85" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="86"/>
-      <c r="D13" s="87">
+      <c r="B13" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="73"/>
+      <c r="D13" s="74">
         <f>SUBTOTAL(109,tbl_InformacionGeneral[GANANCIA BRUTA])</f>
-        <v>87780</v>
-      </c>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="88"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="88"/>
-      <c r="L13" s="88"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="86"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="86"/>
-      <c r="Q13" s="86"/>
-      <c r="R13" s="89">
+        <v>99191.111111111109</v>
+      </c>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="73"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="73"/>
+      <c r="R13" s="76">
         <f>SUBTOTAL(109,tbl_InformacionGeneral[COSTO REAL])</f>
-        <v>33300</v>
+        <v>12000</v>
       </c>
     </row>
   </sheetData>
@@ -4733,7 +5200,7 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="F14:F183 F4:F12">
-    <cfRule type="cellIs" dxfId="72" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4769,10 +5236,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF49EC4-47C7-48DA-845D-A09FB69531BC}">
-  <dimension ref="B2:M33"/>
+  <dimension ref="B2:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4780,7 +5247,7 @@
     <col min="1" max="1" width="5.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
     <col min="3" max="4" width="22.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.88671875" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="6.88671875" style="1" customWidth="1"/>
@@ -4834,10 +5301,18 @@
       <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+      <c r="D3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="10">
+        <v>44623</v>
+      </c>
+      <c r="G3" s="10">
+        <v>44651</v>
+      </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="12"/>
@@ -4855,7 +5330,9 @@
         <v>10</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="7"/>
@@ -4894,10 +5371,16 @@
       <c r="C6" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="E6" s="7"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="F6" s="10">
+        <v>44656</v>
+      </c>
+      <c r="G6" s="10">
+        <v>44686</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="12"/>
@@ -5226,8 +5709,8 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="12"/>
@@ -5264,32 +5747,18 @@
       <c r="M31" s="24"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="24"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B33" s="8"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="25"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5303,7 +5772,7 @@
           <x14:formula1>
             <xm:f>'INFORMACION GENERAL'!$C$4:$C$183</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C33</xm:sqref>
+          <xm:sqref>C3:C32</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5313,421 +5782,338 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50469F63-0CAE-4A44-ABEA-7EA5381AEB51}">
-  <dimension ref="B2:J34"/>
+  <dimension ref="B2:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="50" customWidth="1"/>
-    <col min="3" max="4" width="22.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.5546875" style="1"/>
+    <col min="7" max="7" width="20.21875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" style="100" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="100" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="100" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="100" customWidth="1"/>
+    <col min="12" max="12" width="20.21875" style="66" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="70" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B2" s="91" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="D2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="E2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="F2" s="92" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="92" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="67" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="67" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="67" t="s">
+      <c r="I2" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="63"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
-        <v>38</v>
+      <c r="J2" s="97" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="97" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="102" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="93" t="str">
+        <f>CHOOSE(
+LEN(tbl_Personal[[#This Row],[NOMBRE]]) - LEN(SUBSTITUTE(tbl_Personal[[#This Row],[NOMBRE]]," ","")) + 1,
+LEFT(tbl_Personal[[#This Row],[NOMBRE]]),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1) + 1, 1))</f>
+        <v>PNU</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="64"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="71"/>
+        <v>71</v>
+      </c>
+      <c r="E3" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="7">
+        <f>COUNTIF(tbl_Asignaciones[ASIGNACION],tbl_Personal[[#This Row],[NOMBRE]])</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="10" cm="1">
+        <f t="array" ref="H3">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",MIN(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA DE INICIO]," "))," ")</f>
+        <v>44623</v>
+      </c>
+      <c r="I3" s="10" cm="1">
+        <f t="array" ref="I3">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",MAX(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA FINAL]," "))," ")</f>
+        <v>44686</v>
+      </c>
+      <c r="J3" s="21" cm="1">
+        <f t="array" ref="J3">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",NETWORKDAYS.INTL(MIN(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA FINAL]," ")),MAX(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA DE INICIO]," ")),1)-2," ")</f>
+        <v>2</v>
+      </c>
+      <c r="K3" s="21"/>
+      <c r="L3" s="103" t="str">
+        <f>IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",IF(tbl_Personal[[#This Row],[APROX]]&gt;0,"SI","NO"),"")</f>
+        <v>SI</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="93" t="str">
+        <f>CHOOSE(
+LEN(tbl_Personal[[#This Row],[NOMBRE]]) - LEN(SUBSTITUTE(tbl_Personal[[#This Row],[NOMBRE]]," ","")) + 1,
+LEFT(tbl_Personal[[#This Row],[NOMBRE]]),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1) + 1, 1))</f>
+        <v/>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="64"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="71"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7">
+        <f>COUNTIF(tbl_Asignaciones[ASIGNACION],tbl_Personal[[#This Row],[NOMBRE]])</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="10" t="str" cm="1">
+        <f t="array" ref="H4">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",MIN(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA DE INICIO]," "))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I4" s="10" t="str" cm="1">
+        <f t="array" ref="I4">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",MAX(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA FINAL]," "))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J4" s="98" t="str" cm="1">
+        <f t="array" ref="J4">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",NETWORKDAYS.INTL(MIN(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA FINAL]," ")),MAX(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA DE INICIO]," ")),1)-2," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K4" s="98"/>
+      <c r="L4" s="103" t="str">
+        <f>IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",IF(tbl_Personal[[#This Row],[APROX]]&gt;0,"SI","NO"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="93" t="str">
+        <f>CHOOSE(
+LEN(tbl_Personal[[#This Row],[NOMBRE]]) - LEN(SUBSTITUTE(tbl_Personal[[#This Row],[NOMBRE]]," ","")) + 1,
+LEFT(tbl_Personal[[#This Row],[NOMBRE]]),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1) + 1, 1))</f>
+        <v/>
+      </c>
       <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="D5" s="27" t="str">
+        <f>CHOOSE(
+LEN(tbl_Personal[[#This Row],[NOMBRE]]) - LEN(SUBSTITUTE(tbl_Personal[[#This Row],[NOMBRE]]," ","")) + 1,
+LEFT(tbl_Personal[[#This Row],[NOMBRE]]),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1))</f>
+        <v/>
+      </c>
       <c r="E5" s="7"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="64"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="71"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7">
+        <f>COUNTIF(tbl_Asignaciones[ASIGNACION],tbl_Personal[[#This Row],[NOMBRE]])</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="10" t="str" cm="1">
+        <f t="array" ref="H5">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",MIN(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA DE INICIO]," "))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I5" s="10" t="str" cm="1">
+        <f t="array" ref="I5">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",MAX(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA FINAL]," "))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J5" s="98" t="str" cm="1">
+        <f t="array" ref="J5">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",NETWORKDAYS.INTL(MIN(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA FINAL]," ")),MAX(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA DE INICIO]," ")),1)-2," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K5" s="98"/>
+      <c r="L5" s="103" t="str">
+        <f>IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",IF(tbl_Personal[[#This Row],[APROX]]&gt;0,"SI","NO"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="93" t="str">
+        <f>CHOOSE(
+LEN(tbl_Personal[[#This Row],[NOMBRE]]) - LEN(SUBSTITUTE(tbl_Personal[[#This Row],[NOMBRE]]," ","")) + 1,
+LEFT(tbl_Personal[[#This Row],[NOMBRE]]),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1) + 1, 1))</f>
+        <v/>
+      </c>
       <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="D6" s="27" t="str">
+        <f>CHOOSE(
+LEN(tbl_Personal[[#This Row],[NOMBRE]]) - LEN(SUBSTITUTE(tbl_Personal[[#This Row],[NOMBRE]]," ","")) + 1,
+LEFT(tbl_Personal[[#This Row],[NOMBRE]]),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1))</f>
+        <v/>
+      </c>
       <c r="E6" s="7"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="64"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="71"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="27">
+        <f>COUNTIF(tbl_Asignaciones[ASIGNACION],tbl_Personal[[#This Row],[NOMBRE]])</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="10" t="str" cm="1">
+        <f t="array" ref="H6">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",MIN(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA DE INICIO]," "))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I6" s="10" t="str" cm="1">
+        <f t="array" ref="I6">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",MAX(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA FINAL]," "))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J6" s="98" t="str" cm="1">
+        <f t="array" ref="J6">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",NETWORKDAYS.INTL(MIN(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA FINAL]," ")),MAX(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA DE INICIO]," ")),1)-2," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K6" s="98"/>
+      <c r="L6" s="103" t="str">
+        <f>IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",IF(tbl_Personal[[#This Row],[APROX]]&gt;0,"SI","NO"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="93" t="str">
+        <f>CHOOSE(
+LEN(tbl_Personal[[#This Row],[NOMBRE]]) - LEN(SUBSTITUTE(tbl_Personal[[#This Row],[NOMBRE]]," ","")) + 1,
+LEFT(tbl_Personal[[#This Row],[NOMBRE]]),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1) + 1, 1))</f>
+        <v/>
+      </c>
       <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="27" t="str">
+        <f>CHOOSE(
+LEN(tbl_Personal[[#This Row],[NOMBRE]]) - LEN(SUBSTITUTE(tbl_Personal[[#This Row],[NOMBRE]]," ","")) + 1,
+LEFT(tbl_Personal[[#This Row],[NOMBRE]]),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1))</f>
+        <v/>
+      </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="64"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="71"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="64"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="71"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="64"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="71"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="64"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="71"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="64"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="71"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="64"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="71"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="64"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="71"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="64"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="71"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="64"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="71"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="64"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="71"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="64"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="71"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="64"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="71"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="64"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="71"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="64"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="71"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="64"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="71"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="64"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="71"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="64"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="71"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="64"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="71"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="64"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B26" s="71"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="64"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="71"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="64"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="71"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="64"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="71"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="64"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="71"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="64"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B31" s="71"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="64"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="71"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="45"/>
-      <c r="J32" s="64"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="72"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="69"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="73"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="66"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="27">
+        <f>COUNTIF(tbl_Asignaciones[ASIGNACION],tbl_Personal[[#This Row],[NOMBRE]])</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="10" t="str" cm="1">
+        <f t="array" ref="H7">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",MIN(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA DE INICIO]," "))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I7" s="10" t="str" cm="1">
+        <f t="array" ref="I7">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",MAX(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA FINAL]," "))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J7" s="98" t="str" cm="1">
+        <f t="array" ref="J7">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",NETWORKDAYS.INTL(MIN(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA FINAL]," ")),MAX(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA DE INICIO]," ")),1)-2," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K7" s="98"/>
+      <c r="L7" s="103" t="str">
+        <f>IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",IF(tbl_Personal[[#This Row],[APROX]]&gt;0,"SI","NO"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="95" t="str">
+        <f>CHOOSE(
+LEN(tbl_Personal[[#This Row],[NOMBRE]]) - LEN(SUBSTITUTE(tbl_Personal[[#This Row],[NOMBRE]]," ","")) + 1,
+LEFT(tbl_Personal[[#This Row],[NOMBRE]]),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1) + 1, 1))</f>
+        <v/>
+      </c>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96" t="str">
+        <f>CHOOSE(
+LEN(tbl_Personal[[#This Row],[NOMBRE]]) - LEN(SUBSTITUTE(tbl_Personal[[#This Row],[NOMBRE]]," ","")) + 1,
+LEFT(tbl_Personal[[#This Row],[NOMBRE]]),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1),
+LEFT(tbl_Personal[[#This Row],[NOMBRE]], 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1, 1) &amp; MID(tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]], FIND(" ", tbl_Personal[[#This Row],[NOMBRE]]) + 1) + 1, 1))</f>
+        <v/>
+      </c>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96">
+        <f>COUNTIF(tbl_Asignaciones[ASIGNACION],tbl_Personal[[#This Row],[NOMBRE]])</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="101" t="str" cm="1">
+        <f t="array" ref="H8">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",MIN(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA DE INICIO]," "))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I8" s="101" t="str" cm="1">
+        <f t="array" ref="I8">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",MAX(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA FINAL]," "))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J8" s="99" t="str" cm="1">
+        <f t="array" ref="J8">IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",NETWORKDAYS.INTL(MIN(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA FINAL]," ")),MAX(IF(tbl_Asignaciones[ASIGNACION]=tbl_Personal[[#This Row],[NOMBRE]],tbl_Asignaciones[FECHA DE INICIO]," ")),1)-2," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K8" s="99"/>
+      <c r="L8" s="104" t="str">
+        <f>IF(tbl_Personal[[#This Row],[NOMBRE]]&lt;&gt;"",IF(tbl_Personal[[#This Row],[APROX]]&gt;0,"SI","NO"),"")</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{A788708D-F7BC-4C83-A0F3-836B138613B5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DC41FAE3-CB9B-4F40-982C-3280EA819868}">
+          <x14:formula1>
+            <xm:f>CONFIG!$D$3:$D$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0001A4E8-E3BA-43F0-8AC9-7F2638379F02}">
           <x14:formula1>
             <xm:f>CONFIG!$D$3:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F34</xm:sqref>
+          <xm:sqref>F4:F8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5739,8 +6125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{686CCF2D-7535-41BB-9681-0BE549C0077C}">
   <dimension ref="B2:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6132,7 +6518,7 @@
   <dimension ref="B2:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6376,19 +6762,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="101" t="s">
+      <c r="C2" s="87"/>
+      <c r="D2" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="102"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="99" t="s">
+      <c r="E2" s="89"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="100"/>
+      <c r="H2" s="87"/>
       <c r="I2" s="12">
         <f>SUM(M5:M200)</f>
         <v>3840</v>
@@ -6625,7 +7011,7 @@
   <dimension ref="B2:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6644,7 +7030,7 @@
         <v>20</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>50</v>
@@ -6656,7 +7042,7 @@
         <v>FIRMA DIGITAL</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" s="7"/>
     </row>
@@ -6665,7 +7051,7 @@
         <v>GEOLOCALIZACION</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -6674,20 +7060,22 @@
         <v>0</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>